<commit_message>
Processed .geoJSONs to be mutually compatible for visualization.
</commit_message>
<xml_diff>
--- a/ZoningAtlas/raw_data/Excel_workbooks/Orange_Chelsea_features.xlsx
+++ b/ZoningAtlas/raw_data/Excel_workbooks/Orange_Chelsea_features.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ybird/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ybird/ZoningAtlas/VT_Zoning_Atlas/ZoningAtlas/raw_data/Excel_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051DBEBF-F346-EE4B-8119-2D817A5ACB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3C0CDB-083F-C047-BB38-A2FC379E09F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32100" windowHeight="15460" activeTab="1" xr2:uid="{FC763E2B-1BB8-D248-8DD1-F66FE797A262}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32100" windowHeight="15460" xr2:uid="{FC763E2B-1BB8-D248-8DD1-F66FE797A262}"/>
   </bookViews>
   <sheets>
     <sheet name="Districts" sheetId="1" r:id="rId1"/>
@@ -496,231 +496,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="126">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="94">
     <dxf>
       <fill>
         <patternFill>
@@ -1691,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4BA41B-4280-B747-9B6E-C79D73F6A3E5}">
   <dimension ref="A1:M144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
@@ -5617,544 +5393,454 @@
   <mergeCells count="1">
     <mergeCell ref="B113:M113"/>
   </mergeCells>
-  <conditionalFormatting sqref="B34:B35 D34:D35 F34:F49 H34:H49 J35 B36:E41 G36:G41 I36:I41 K36:K41 J37 L37 J42:J49 L42:L49 L34:M35 M36:M41 B42:B48 D42:D48 B49:E49 G49 I49 K49 M49">
-    <cfRule type="expression" dxfId="125" priority="288">
+  <conditionalFormatting sqref="B34:B35 D34:D35 L34:M35 F34:F49 H34:H49 J35 B36:E41 G36:G41 I36:I41 K36:K41 M36:M41 J37 L37 B42:B48 D42:D48 J42:J49 L42:L49 B49:E49 G49 I49 K49 M49">
+    <cfRule type="expression" dxfId="93" priority="288">
       <formula>OR(B$12="", B$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51:B52 D51:D52 F51:F54 H51:H69 J52 B53:E54 J54 L54 C55:E58 B59:E62 F59:F69 J59:J69 L59:L69 B63:B64 D63:D64 L51:M52 B65:E69 G65:G69 I65:I69 K65:K69 M65:M69 G53:G62 I53:I62 K53:K62 M53:M62">
-    <cfRule type="expression" dxfId="124" priority="287" stopIfTrue="1">
+  <conditionalFormatting sqref="B51:B52 D51:D52 L51:M52 F51:F54 H51:H69 J52 B53:E54 G53:G62 I53:I62 K53:K62 M53:M62 J54 L54 C55:E58 B59:E62 F59:F69 J59:J69 L59:L69 B63:B64 D63:D64 B65:E69 G65:G69 I65:I69 K65:K69 M65:M69">
+    <cfRule type="expression" dxfId="92" priority="287" stopIfTrue="1">
       <formula>OR(B$13="", B$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:B58">
-    <cfRule type="expression" dxfId="123" priority="53">
+    <cfRule type="expression" dxfId="91" priority="53">
       <formula>OR(B$12="", B$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:C26 E26:F26 B27:F32 B21:M25 G26:M32">
-    <cfRule type="expression" dxfId="122" priority="289" stopIfTrue="1">
+  <conditionalFormatting sqref="B114:B121 D114:D121 F114:F121 H114:H121 J114:J121 L114:L121">
+    <cfRule type="expression" dxfId="90" priority="284" stopIfTrue="1">
+      <formula>OR(B$17="", B$17="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B123:B132 D123:D132 F123:F132 H123:H132 J123:J132 L123:L132">
+    <cfRule type="expression" dxfId="89" priority="283">
+      <formula>OR(B$16="", B$16="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B134:B137 D134:D137 F134:F137 H134:H137 J134:J137 L134:L137">
+    <cfRule type="expression" dxfId="88" priority="282" stopIfTrue="1">
+      <formula>OR(B$18="Prohibited", B$18="")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:M25 B26:C26 E26:F26 G26:M32 B27:F32">
+    <cfRule type="expression" dxfId="87" priority="289" stopIfTrue="1">
       <formula>OR(B$11="", B$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73:C78">
-    <cfRule type="expression" dxfId="121" priority="281" stopIfTrue="1">
+  <conditionalFormatting sqref="C42:C48">
+    <cfRule type="expression" dxfId="86" priority="50" stopIfTrue="1">
+      <formula>OR(C$11="", C$11="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73:C82">
+    <cfRule type="expression" dxfId="85" priority="44" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C94:C99">
-    <cfRule type="expression" dxfId="120" priority="279" stopIfTrue="1">
+  <conditionalFormatting sqref="C85:C89">
+    <cfRule type="expression" dxfId="84" priority="38" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C115">
-    <cfRule type="expression" dxfId="118" priority="272" stopIfTrue="1">
+  <conditionalFormatting sqref="C94:C103">
+    <cfRule type="expression" dxfId="83" priority="32" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C106:C110">
+    <cfRule type="expression" dxfId="82" priority="25" stopIfTrue="1">
+      <formula>OR(C$13="", C$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C111">
+    <cfRule type="expression" dxfId="81" priority="26">
+      <formula>OR(C$14="", C$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C115:C120">
+    <cfRule type="expression" dxfId="80" priority="13" stopIfTrue="1">
+      <formula>OR(C$13="", C$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C121">
+    <cfRule type="expression" dxfId="79" priority="14">
+      <formula>OR(C$14="", C$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C127:C128">
-    <cfRule type="expression" dxfId="116" priority="270" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="270" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C130:C132">
-    <cfRule type="expression" dxfId="115" priority="267" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="267" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C135:C136">
-    <cfRule type="expression" dxfId="114" priority="265" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="265" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73:E78">
-    <cfRule type="expression" dxfId="113" priority="111" stopIfTrue="1">
+  <conditionalFormatting sqref="E42:E48">
+    <cfRule type="expression" dxfId="75" priority="49" stopIfTrue="1">
+      <formula>OR(E$11="", E$11="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E73:E82">
+    <cfRule type="expression" dxfId="74" priority="43" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E94:E99">
-    <cfRule type="expression" dxfId="112" priority="109" stopIfTrue="1">
+  <conditionalFormatting sqref="E85:E89">
+    <cfRule type="expression" dxfId="73" priority="37" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E115">
-    <cfRule type="expression" dxfId="110" priority="107" stopIfTrue="1">
+  <conditionalFormatting sqref="E94:E103">
+    <cfRule type="expression" dxfId="72" priority="31" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E106:E110">
+    <cfRule type="expression" dxfId="71" priority="23" stopIfTrue="1">
+      <formula>OR(E$13="", E$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E111">
+    <cfRule type="expression" dxfId="70" priority="24">
+      <formula>OR(E$14="", E$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E115:E120">
+    <cfRule type="expression" dxfId="69" priority="11" stopIfTrue="1">
+      <formula>OR(E$13="", E$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E121">
+    <cfRule type="expression" dxfId="68" priority="12">
+      <formula>OR(E$14="", E$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E127:E128">
-    <cfRule type="expression" dxfId="108" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="106" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130:E132">
-    <cfRule type="expression" dxfId="107" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="105" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E135:E136">
-    <cfRule type="expression" dxfId="106" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="104" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55:F58">
-    <cfRule type="expression" dxfId="105" priority="79">
+    <cfRule type="expression" dxfId="64" priority="79">
       <formula>OR(F$12="", F$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G73:G78">
-    <cfRule type="expression" dxfId="104" priority="103" stopIfTrue="1">
+  <conditionalFormatting sqref="G42:G48">
+    <cfRule type="expression" dxfId="63" priority="48" stopIfTrue="1">
+      <formula>OR(G$11="", G$11="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G73:G82">
+    <cfRule type="expression" dxfId="62" priority="42" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G94:G99">
-    <cfRule type="expression" dxfId="103" priority="101" stopIfTrue="1">
+  <conditionalFormatting sqref="G85:G89">
+    <cfRule type="expression" dxfId="61" priority="36" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G115">
-    <cfRule type="expression" dxfId="101" priority="99" stopIfTrue="1">
+  <conditionalFormatting sqref="G94:G103">
+    <cfRule type="expression" dxfId="60" priority="30" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G106:G110">
+    <cfRule type="expression" dxfId="59" priority="21" stopIfTrue="1">
+      <formula>OR(G$13="", G$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G111">
+    <cfRule type="expression" dxfId="58" priority="22">
+      <formula>OR(G$14="", G$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G115:G120">
+    <cfRule type="expression" dxfId="57" priority="9" stopIfTrue="1">
+      <formula>OR(G$13="", G$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G121">
+    <cfRule type="expression" dxfId="56" priority="10">
+      <formula>OR(G$14="", G$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G127:G128">
-    <cfRule type="expression" dxfId="99" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="98" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G130:G132">
-    <cfRule type="expression" dxfId="98" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="97" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G135:G136">
-    <cfRule type="expression" dxfId="97" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="96" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I73:I78">
-    <cfRule type="expression" dxfId="96" priority="95" stopIfTrue="1">
+  <conditionalFormatting sqref="I42:I48">
+    <cfRule type="expression" dxfId="52" priority="47" stopIfTrue="1">
+      <formula>OR(I$11="", I$11="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I73:I82">
+    <cfRule type="expression" dxfId="51" priority="41" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I94:I99">
-    <cfRule type="expression" dxfId="95" priority="93" stopIfTrue="1">
+  <conditionalFormatting sqref="I85:I89">
+    <cfRule type="expression" dxfId="50" priority="35" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I115">
-    <cfRule type="expression" dxfId="93" priority="91" stopIfTrue="1">
+  <conditionalFormatting sqref="I94:I103">
+    <cfRule type="expression" dxfId="49" priority="29" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I106:I110">
+    <cfRule type="expression" dxfId="48" priority="19" stopIfTrue="1">
+      <formula>OR(I$13="", I$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I111">
+    <cfRule type="expression" dxfId="47" priority="20">
+      <formula>OR(I$14="", I$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I115:I120">
+    <cfRule type="expression" dxfId="46" priority="7" stopIfTrue="1">
+      <formula>OR(I$13="", I$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I121">
+    <cfRule type="expression" dxfId="45" priority="8">
+      <formula>OR(I$14="", I$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I127:I128">
-    <cfRule type="expression" dxfId="91" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="90" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I130:I132">
-    <cfRule type="expression" dxfId="90" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="89" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I135:I136">
-    <cfRule type="expression" dxfId="89" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="88" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34">
-    <cfRule type="expression" dxfId="88" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="78" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36">
-    <cfRule type="expression" dxfId="87" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="76" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:J41">
-    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="72" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51">
-    <cfRule type="expression" dxfId="85" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="77" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J53">
-    <cfRule type="expression" dxfId="84" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="75" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55:J58">
-    <cfRule type="expression" dxfId="83" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="70" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:J72 L71:L72 B71:B89 D71:D90 F71:F90 H71:H90 J74 L74 J79:J90 L79:L90 B90:C90 E90 G90 I90 K90 M90">
-    <cfRule type="expression" dxfId="82" priority="286">
+    <cfRule type="expression" dxfId="35" priority="286">
       <formula>OR(B$14="", B$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73">
-    <cfRule type="expression" dxfId="81" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="74" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:J78">
-    <cfRule type="expression" dxfId="80" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="69" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92:J93 L92:L93 B92:B111 D92:D111 F92:F111 H92:H111 J95 L95 J100:J111 L100:L111">
-    <cfRule type="expression" dxfId="79" priority="285" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="285" stopIfTrue="1">
       <formula>OR(B$15="", B$15="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J94">
-    <cfRule type="expression" dxfId="78" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="73" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J96:J99">
-    <cfRule type="expression" dxfId="77" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="52" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K73:K78">
-    <cfRule type="expression" dxfId="76" priority="87" stopIfTrue="1">
+  <conditionalFormatting sqref="K42:K48">
+    <cfRule type="expression" dxfId="29" priority="46" stopIfTrue="1">
+      <formula>OR(K$11="", K$11="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73:K82">
+    <cfRule type="expression" dxfId="28" priority="40" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K94:K99">
-    <cfRule type="expression" dxfId="75" priority="85" stopIfTrue="1">
+  <conditionalFormatting sqref="K85:K89">
+    <cfRule type="expression" dxfId="27" priority="34" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K115">
-    <cfRule type="expression" dxfId="73" priority="83" stopIfTrue="1">
+  <conditionalFormatting sqref="K94:K103">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K106:K110">
+    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+      <formula>OR(K$13="", K$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K111">
+    <cfRule type="expression" dxfId="24" priority="18">
+      <formula>OR(K$14="", K$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K115:K120">
+    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
+      <formula>OR(K$13="", K$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K121">
+    <cfRule type="expression" dxfId="22" priority="6">
+      <formula>OR(K$14="", K$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K127:K128">
+    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
+      <formula>OR(K$13="", K$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K130:K132">
-    <cfRule type="expression" dxfId="70" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="81" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K135:K136">
-    <cfRule type="expression" dxfId="69" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="80" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L36">
-    <cfRule type="expression" dxfId="68" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="68" stopIfTrue="1">
       <formula>OR(L$11="", L$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L41">
-    <cfRule type="expression" dxfId="67" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="67" stopIfTrue="1">
       <formula>OR(L$11="", L$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53">
-    <cfRule type="expression" dxfId="66" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="66" stopIfTrue="1">
       <formula>OR(L$11="", L$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:L58">
-    <cfRule type="expression" dxfId="65" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="65" stopIfTrue="1">
       <formula>OR(L$11="", L$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L73">
-    <cfRule type="expression" dxfId="64" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="63" stopIfTrue="1">
       <formula>OR(L$11="", L$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L75:L78">
-    <cfRule type="expression" dxfId="63" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="62" stopIfTrue="1">
       <formula>OR(L$11="", L$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L94">
-    <cfRule type="expression" dxfId="62" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="59" stopIfTrue="1">
       <formula>OR(L$11="", L$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L96:L99">
-    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="51" stopIfTrue="1">
       <formula>OR(L$11="", L$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M73:M78">
-    <cfRule type="expression" dxfId="60" priority="64" stopIfTrue="1">
+  <conditionalFormatting sqref="M42:M48">
+    <cfRule type="expression" dxfId="10" priority="45" stopIfTrue="1">
+      <formula>OR(M$11="", M$11="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M73:M82">
+    <cfRule type="expression" dxfId="9" priority="39" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M94:M99">
-    <cfRule type="expression" dxfId="59" priority="60" stopIfTrue="1">
+  <conditionalFormatting sqref="M85:M89">
+    <cfRule type="expression" dxfId="8" priority="33" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M115">
-    <cfRule type="expression" dxfId="57" priority="57" stopIfTrue="1">
+  <conditionalFormatting sqref="M94:M103">
+    <cfRule type="expression" dxfId="7" priority="27" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M130:M132">
-    <cfRule type="expression" dxfId="54" priority="55" stopIfTrue="1">
+  <conditionalFormatting sqref="M106:M110">
+    <cfRule type="expression" dxfId="6" priority="15" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M135:M136">
-    <cfRule type="expression" dxfId="53" priority="54" stopIfTrue="1">
+  <conditionalFormatting sqref="M111">
+    <cfRule type="expression" dxfId="5" priority="16">
+      <formula>OR(M$14="", M$14="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M115:M120">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B114:B121 D114:D121 F114:F121 H114:H121 J114:J121 L114:L121">
-    <cfRule type="expression" dxfId="52" priority="284" stopIfTrue="1">
-      <formula>OR(B$17="", B$17="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B123:B132 D123:D132 F123:F132 H123:H132 J123:J132 L123:L132">
-    <cfRule type="expression" dxfId="51" priority="283">
-      <formula>OR(B$16="", B$16="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B134:B137 D134:D137 F134:F137 H134:H137 J134:J137 L134:L137">
-    <cfRule type="expression" dxfId="50" priority="282" stopIfTrue="1">
-      <formula>OR(B$18="Prohibited", B$18="")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42:C48">
-    <cfRule type="expression" dxfId="49" priority="50" stopIfTrue="1">
-      <formula>OR(C$11="", C$11="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42:E48">
-    <cfRule type="expression" dxfId="48" priority="49" stopIfTrue="1">
-      <formula>OR(E$11="", E$11="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G42:G48">
-    <cfRule type="expression" dxfId="47" priority="48" stopIfTrue="1">
-      <formula>OR(G$11="", G$11="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42:I48">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
-      <formula>OR(I$11="", I$11="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K42:K48">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
-      <formula>OR(K$11="", K$11="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M42:M48">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
-      <formula>OR(M$11="", M$11="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C79:C82">
-    <cfRule type="expression" dxfId="43" priority="44" stopIfTrue="1">
-      <formula>OR(C$13="", C$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E79:E82">
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
-      <formula>OR(E$13="", E$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G79:G82">
-    <cfRule type="expression" dxfId="41" priority="42" stopIfTrue="1">
-      <formula>OR(G$13="", G$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I79:I82">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
-      <formula>OR(I$13="", I$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K79:K82">
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
-      <formula>OR(K$13="", K$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M79:M82">
-    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
-      <formula>OR(M$13="", M$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C85:C89">
-    <cfRule type="expression" dxfId="37" priority="38" stopIfTrue="1">
-      <formula>OR(C$13="", C$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E89">
-    <cfRule type="expression" dxfId="36" priority="37" stopIfTrue="1">
-      <formula>OR(E$13="", E$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G85:G89">
-    <cfRule type="expression" dxfId="35" priority="36" stopIfTrue="1">
-      <formula>OR(G$13="", G$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I85:I89">
-    <cfRule type="expression" dxfId="34" priority="35" stopIfTrue="1">
-      <formula>OR(I$13="", I$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K85:K89">
-    <cfRule type="expression" dxfId="33" priority="34" stopIfTrue="1">
-      <formula>OR(K$13="", K$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M85:M89">
-    <cfRule type="expression" dxfId="32" priority="33" stopIfTrue="1">
-      <formula>OR(M$13="", M$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C100:C103">
-    <cfRule type="expression" dxfId="31" priority="32" stopIfTrue="1">
-      <formula>OR(C$13="", C$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E100:E103">
-    <cfRule type="expression" dxfId="30" priority="31" stopIfTrue="1">
-      <formula>OR(E$13="", E$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G100:G103">
-    <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
-      <formula>OR(G$13="", G$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I100:I103">
-    <cfRule type="expression" dxfId="28" priority="29" stopIfTrue="1">
-      <formula>OR(I$13="", I$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K100:K103">
-    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
-      <formula>OR(K$13="", K$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M100:M103">
-    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
-      <formula>OR(M$13="", M$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C111">
-    <cfRule type="expression" dxfId="25" priority="26">
-      <formula>OR(C$14="", C$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C106:C110">
-    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
-      <formula>OR(C$13="", C$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E111">
-    <cfRule type="expression" dxfId="23" priority="24">
-      <formula>OR(E$14="", E$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E106:E110">
-    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
-      <formula>OR(E$13="", E$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G111">
-    <cfRule type="expression" dxfId="21" priority="22">
-      <formula>OR(G$14="", G$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G106:G110">
-    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
-      <formula>OR(G$13="", G$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I111">
-    <cfRule type="expression" dxfId="19" priority="20">
-      <formula>OR(I$14="", I$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I106:I110">
-    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
-      <formula>OR(I$13="", I$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K111">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>OR(K$14="", K$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K106:K110">
-    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
-      <formula>OR(K$13="", K$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M111">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>OR(M$14="", M$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M106:M110">
-    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
-      <formula>OR(M$13="", M$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C121">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>OR(C$14="", C$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C116:C120">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
-      <formula>OR(C$13="", C$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E121">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>OR(E$14="", E$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E116:E120">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>OR(E$13="", E$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G121">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>OR(G$14="", G$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G116:G120">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
-      <formula>OR(G$13="", G$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I121">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>OR(I$14="", I$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I116:I120">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>OR(I$13="", I$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K121">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>OR(K$14="", K$14="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K116:K120">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M121">
@@ -6162,18 +5848,18 @@
       <formula>OR(M$14="", M$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M116:M120">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="M127:M128">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K127:K128">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>OR(K$13="", K$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M127:M128">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="M130:M132">
+    <cfRule type="expression" dxfId="1" priority="55" stopIfTrue="1">
+      <formula>OR(M$13="", M$13="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M135:M136">
+    <cfRule type="expression" dxfId="0" priority="54" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6293,8 +5979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05389331-E65F-9747-B96F-F1FC2DF92AD8}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6396,24 +6082,24 @@
         <v>FHO</v>
       </c>
       <c r="C12" t="str">
+        <f>Districts!D1</f>
+        <v>IND</v>
+      </c>
+      <c r="D12" t="str">
+        <f>Districts!F1</f>
+        <v>MU</v>
+      </c>
+      <c r="E12" t="str">
         <f>Districts!H1</f>
         <v>RR</v>
       </c>
-      <c r="D12" t="str">
+      <c r="F12" t="str">
+        <f>Districts!J1</f>
+        <v>VIL</v>
+      </c>
+      <c r="G12" t="str">
         <f>Districts!L1</f>
         <v>WHPO</v>
-      </c>
-      <c r="E12" t="e">
-        <f>Districts!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F12" t="e">
-        <f>Districts!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G12" t="e">
-        <f>Districts!#REF!</f>
-        <v>#REF!</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>